<commit_message>
Added white blood cells
Added total and each white blood cell type, their functions (both total and percentage), updated its data and the documentation.
</commit_message>
<xml_diff>
--- a/Background_Data/hemogram.xlsx
+++ b/Background_Data/hemogram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Git Repositories\UFTM-BioStat-DataBase\Background_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0C5217-6C03-4A22-83E1-6637AEC141DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397AEB96-B1DC-4F42-84BC-4CDE88FA65CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{ACC5E948-CBA1-493D-8CCB-6A4BFE567CAB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>min</t>
   </si>
@@ -175,6 +175,36 @@
   </si>
   <si>
     <t>mcv_sd</t>
+  </si>
+  <si>
+    <t>neutrophils_mean</t>
+  </si>
+  <si>
+    <t>neutrophils_sd</t>
+  </si>
+  <si>
+    <t>lymphocytes_mean</t>
+  </si>
+  <si>
+    <t>lymphocytes_sd</t>
+  </si>
+  <si>
+    <t>monocytes_mean</t>
+  </si>
+  <si>
+    <t>monocytes_sd</t>
+  </si>
+  <si>
+    <t>eosinophils_mean</t>
+  </si>
+  <si>
+    <t>eosinophils_sd</t>
+  </si>
+  <si>
+    <t>basophils_mean</t>
+  </si>
+  <si>
+    <t>basophils_sd</t>
   </si>
 </sst>
 </file>
@@ -526,11 +556,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A850E237-D5E7-4798-BE04-50C11F2744C0}">
-  <dimension ref="A1:AE10"/>
+  <dimension ref="A1:AO10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L9" sqref="K9:L9"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +568,7 @@
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -585,55 +615,85 @@
         <v>23</v>
       </c>
       <c r="P1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R1" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>25</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>26</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>27</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X1" t="s">
         <v>28</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Y1" t="s">
         <v>29</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Z1" t="s">
         <v>30</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AA1" t="s">
         <v>31</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AB1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD1" t="s">
         <v>32</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AE1" t="s">
         <v>33</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AF1" t="s">
         <v>34</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AG1" t="s">
         <v>35</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AH1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>36</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AK1" t="s">
         <v>37</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AL1" t="s">
         <v>38</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AM1" t="s">
         <v>39</v>
       </c>
+      <c r="AN1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -680,55 +740,95 @@
         <v>6000</v>
       </c>
       <c r="P2">
+        <f>AVERAGE(N2:O2)</f>
+        <v>4000</v>
+      </c>
+      <c r="Q2">
+        <f>(O2-P2)/2.5</f>
+        <v>800</v>
+      </c>
+      <c r="R2">
         <v>40</v>
       </c>
-      <c r="Q2">
+      <c r="S2">
         <v>70</v>
       </c>
-      <c r="R2">
+      <c r="T2">
         <v>3000</v>
       </c>
-      <c r="S2">
+      <c r="U2">
         <v>10000</v>
       </c>
-      <c r="T2">
+      <c r="V2">
+        <f>AVERAGE(T2:U2)</f>
+        <v>6500</v>
+      </c>
+      <c r="W2">
+        <f>(U2-V2)/2.5</f>
+        <v>1400</v>
+      </c>
+      <c r="X2">
         <v>2</v>
       </c>
-      <c r="U2">
+      <c r="Y2">
         <v>8</v>
       </c>
-      <c r="V2">
+      <c r="Z2">
         <v>200</v>
       </c>
-      <c r="W2">
+      <c r="AA2">
         <v>1200</v>
       </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
+      <c r="AB2">
+        <f>AVERAGE(Z2:AA2)</f>
+        <v>700</v>
+      </c>
+      <c r="AC2">
+        <f>(AA2-AB2)/2.5</f>
+        <v>200</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
         <v>7</v>
       </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AA2">
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
         <v>800</v>
       </c>
-      <c r="AB2">
-        <v>0</v>
-      </c>
-      <c r="AC2">
+      <c r="AH2">
+        <f>AVERAGE(AF2:AG2)</f>
+        <v>400</v>
+      </c>
+      <c r="AI2">
+        <f>(AG2-AH2)/2.5</f>
+        <v>160</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
         <v>3</v>
       </c>
-      <c r="AD2">
-        <v>0</v>
-      </c>
-      <c r="AE2">
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
         <v>300</v>
       </c>
+      <c r="AN2">
+        <f>AVERAGE(AL2:AM2)</f>
+        <v>150</v>
+      </c>
+      <c r="AO2">
+        <f>(AM2-AN2)/2.5</f>
+        <v>60</v>
+      </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -757,7 +857,7 @@
         <v>6</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:S4" si="0">J2</f>
+        <f t="shared" ref="J3:O4" si="0">J2</f>
         <v>6000</v>
       </c>
       <c r="K3">
@@ -781,71 +881,111 @@
         <v>6000</v>
       </c>
       <c r="P3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="P3:P10" si="1">AVERAGE(N3:O3)</f>
+        <v>4000</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q10" si="2">(O3-P3)/2.5</f>
+        <v>800</v>
+      </c>
+      <c r="R3">
+        <f>R2</f>
         <v>40</v>
       </c>
-      <c r="Q3">
-        <f t="shared" si="0"/>
+      <c r="S3">
+        <f>S2</f>
         <v>70</v>
       </c>
-      <c r="R3">
-        <f t="shared" si="0"/>
+      <c r="T3">
+        <f>T2</f>
         <v>3000</v>
       </c>
-      <c r="S3">
-        <f t="shared" si="0"/>
+      <c r="U3">
+        <f>U2</f>
         <v>10000</v>
       </c>
-      <c r="T3">
-        <f t="shared" ref="T3:AC4" si="1">T2</f>
+      <c r="V3">
+        <f t="shared" ref="V3:V10" si="3">AVERAGE(T3:U3)</f>
+        <v>6500</v>
+      </c>
+      <c r="W3">
+        <f t="shared" ref="W3:W10" si="4">(U3-V3)/2.5</f>
+        <v>1400</v>
+      </c>
+      <c r="X3">
+        <f t="shared" ref="X3:AG4" si="5">X2</f>
         <v>2</v>
       </c>
-      <c r="U3">
-        <f t="shared" si="1"/>
+      <c r="Y3">
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="V3">
-        <f t="shared" si="1"/>
+      <c r="Z3">
+        <f t="shared" si="5"/>
         <v>200</v>
       </c>
-      <c r="W3">
-        <f t="shared" si="1"/>
+      <c r="AA3">
+        <f t="shared" si="5"/>
         <v>1200</v>
       </c>
-      <c r="X3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Y3">
-        <f t="shared" si="1"/>
+      <c r="AB3">
+        <f t="shared" ref="AB3:AB10" si="6">AVERAGE(Z3:AA3)</f>
+        <v>700</v>
+      </c>
+      <c r="AC3">
+        <f t="shared" ref="AC3:AC10" si="7">(AA3-AB3)/2.5</f>
+        <v>200</v>
+      </c>
+      <c r="AD3">
+        <f>AD2</f>
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <f>AE2</f>
         <v>7</v>
       </c>
-      <c r="Z3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AA3">
-        <f t="shared" si="1"/>
+      <c r="AF3">
+        <f>AF2</f>
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <f>AG2</f>
         <v>800</v>
       </c>
-      <c r="AB3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AC3">
-        <f t="shared" si="1"/>
+      <c r="AH3">
+        <f t="shared" ref="AH3:AH10" si="8">AVERAGE(AF3:AG3)</f>
+        <v>400</v>
+      </c>
+      <c r="AI3">
+        <f t="shared" ref="AI3:AI10" si="9">(AG3-AH3)/2.5</f>
+        <v>160</v>
+      </c>
+      <c r="AJ3">
+        <f>AJ2</f>
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <f>AK2</f>
         <v>3</v>
       </c>
-      <c r="AD3">
-        <f t="shared" ref="AD3:AM4" si="2">AD2</f>
-        <v>0</v>
-      </c>
-      <c r="AE3">
-        <f t="shared" si="2"/>
+      <c r="AL3">
+        <f t="shared" ref="AL3:AM4" si="10">AL2</f>
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <f t="shared" si="10"/>
         <v>300</v>
       </c>
+      <c r="AN3">
+        <f t="shared" ref="AN3:AN10" si="11">AVERAGE(AL3:AM3)</f>
+        <v>150</v>
+      </c>
+      <c r="AO3">
+        <f t="shared" ref="AO3:AO10" si="12">(AM3-AN3)/2.5</f>
+        <v>60</v>
+      </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -898,71 +1038,111 @@
         <v>6000</v>
       </c>
       <c r="P4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>4000</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="2"/>
+        <v>800</v>
+      </c>
+      <c r="R4">
+        <f>R3</f>
         <v>40</v>
       </c>
-      <c r="Q4">
-        <f t="shared" si="0"/>
+      <c r="S4">
+        <f>S3</f>
         <v>70</v>
       </c>
-      <c r="R4">
-        <f t="shared" si="0"/>
+      <c r="T4">
+        <f>T3</f>
         <v>3000</v>
       </c>
-      <c r="S4">
-        <f t="shared" si="0"/>
+      <c r="U4">
+        <f>U3</f>
         <v>10000</v>
       </c>
-      <c r="T4">
-        <f t="shared" si="1"/>
+      <c r="V4">
+        <f t="shared" si="3"/>
+        <v>6500</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="4"/>
+        <v>1400</v>
+      </c>
+      <c r="X4">
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="U4">
-        <f t="shared" si="1"/>
+      <c r="Y4">
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="V4">
-        <f t="shared" si="1"/>
+      <c r="Z4">
+        <f t="shared" si="5"/>
         <v>200</v>
       </c>
-      <c r="W4">
-        <f t="shared" si="1"/>
+      <c r="AA4">
+        <f t="shared" si="5"/>
         <v>1200</v>
       </c>
-      <c r="X4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <f t="shared" si="1"/>
+      <c r="AB4">
+        <f t="shared" si="6"/>
+        <v>700</v>
+      </c>
+      <c r="AC4">
+        <f t="shared" si="7"/>
+        <v>200</v>
+      </c>
+      <c r="AD4">
+        <f>AD3</f>
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <f>AE3</f>
         <v>7</v>
       </c>
-      <c r="Z4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AA4">
-        <f t="shared" si="1"/>
+      <c r="AF4">
+        <f>AF3</f>
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <f>AG3</f>
         <v>800</v>
       </c>
-      <c r="AB4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AC4">
-        <f t="shared" si="1"/>
+      <c r="AH4">
+        <f t="shared" si="8"/>
+        <v>400</v>
+      </c>
+      <c r="AI4">
+        <f t="shared" si="9"/>
+        <v>160</v>
+      </c>
+      <c r="AJ4">
+        <f>AJ3</f>
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <f>AK3</f>
         <v>3</v>
       </c>
-      <c r="AD4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AE4">
-        <f t="shared" si="2"/>
+      <c r="AL4">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <f t="shared" si="10"/>
         <v>300</v>
       </c>
+      <c r="AN4">
+        <f t="shared" si="11"/>
+        <v>150</v>
+      </c>
+      <c r="AO4">
+        <f t="shared" si="12"/>
+        <v>60</v>
+      </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1009,55 +1189,95 @@
         <v>4000</v>
       </c>
       <c r="P5">
+        <f t="shared" si="1"/>
+        <v>2500</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="2"/>
+        <v>600</v>
+      </c>
+      <c r="R5">
         <v>50</v>
       </c>
-      <c r="Q5">
+      <c r="S5">
         <v>80</v>
       </c>
-      <c r="R5">
+      <c r="T5">
         <v>3000</v>
       </c>
-      <c r="S5">
+      <c r="U5">
         <v>10000</v>
       </c>
-      <c r="T5">
+      <c r="V5">
+        <f t="shared" si="3"/>
+        <v>6500</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="4"/>
+        <v>1400</v>
+      </c>
+      <c r="X5">
         <v>2</v>
       </c>
-      <c r="U5">
+      <c r="Y5">
         <v>10</v>
       </c>
-      <c r="V5">
+      <c r="Z5">
         <v>100</v>
       </c>
-      <c r="W5">
+      <c r="AA5">
         <v>1000</v>
       </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="Y5">
+      <c r="AB5">
+        <f t="shared" si="6"/>
+        <v>550</v>
+      </c>
+      <c r="AC5">
+        <f t="shared" si="7"/>
+        <v>180</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
         <v>7</v>
       </c>
-      <c r="Z5">
-        <v>0</v>
-      </c>
-      <c r="AA5">
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
         <v>700</v>
       </c>
-      <c r="AB5">
-        <v>0</v>
-      </c>
-      <c r="AC5">
+      <c r="AH5">
+        <f t="shared" si="8"/>
+        <v>350</v>
+      </c>
+      <c r="AI5">
+        <f t="shared" si="9"/>
+        <v>140</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
         <v>3</v>
       </c>
-      <c r="AD5">
-        <v>0</v>
-      </c>
-      <c r="AE5">
+      <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5">
         <v>300</v>
       </c>
+      <c r="AN5">
+        <f t="shared" si="11"/>
+        <v>150</v>
+      </c>
+      <c r="AO5">
+        <f t="shared" si="12"/>
+        <v>60</v>
+      </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1104,55 +1324,95 @@
         <v>6000</v>
       </c>
       <c r="P6">
+        <f t="shared" si="1"/>
+        <v>3500</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="2"/>
+        <v>1000</v>
+      </c>
+      <c r="R6">
         <v>40</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <v>70</v>
       </c>
-      <c r="R6">
+      <c r="T6">
         <v>2000</v>
       </c>
-      <c r="S6">
+      <c r="U6">
         <v>8000</v>
       </c>
-      <c r="T6">
+      <c r="V6">
+        <f t="shared" si="3"/>
+        <v>5000</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="4"/>
+        <v>1200</v>
+      </c>
+      <c r="X6">
         <v>2</v>
       </c>
-      <c r="U6">
+      <c r="Y6">
         <v>10</v>
       </c>
-      <c r="V6">
+      <c r="Z6">
         <v>100</v>
       </c>
-      <c r="W6">
+      <c r="AA6">
         <v>1000</v>
       </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
-      <c r="Y6">
+      <c r="AB6">
+        <f t="shared" si="6"/>
+        <v>550</v>
+      </c>
+      <c r="AC6">
+        <f t="shared" si="7"/>
+        <v>180</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
         <v>7</v>
       </c>
-      <c r="Z6">
-        <v>0</v>
-      </c>
-      <c r="AA6">
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
         <v>600</v>
       </c>
-      <c r="AB6">
-        <v>0</v>
-      </c>
-      <c r="AC6">
+      <c r="AH6">
+        <f t="shared" si="8"/>
+        <v>300</v>
+      </c>
+      <c r="AI6">
+        <f t="shared" si="9"/>
+        <v>120</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
         <v>3</v>
       </c>
-      <c r="AD6">
-        <v>0</v>
-      </c>
-      <c r="AE6">
+      <c r="AL6">
+        <v>0</v>
+      </c>
+      <c r="AM6">
         <v>300</v>
       </c>
+      <c r="AN6">
+        <f t="shared" si="11"/>
+        <v>150</v>
+      </c>
+      <c r="AO6">
+        <f t="shared" si="12"/>
+        <v>60</v>
+      </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1199,55 +1459,95 @@
         <v>6000</v>
       </c>
       <c r="P7">
+        <f t="shared" si="1"/>
+        <v>3700</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="2"/>
+        <v>920</v>
+      </c>
+      <c r="R7">
         <v>30</v>
       </c>
-      <c r="Q7">
+      <c r="S7">
         <v>60</v>
       </c>
-      <c r="R7">
+      <c r="T7">
         <v>1600</v>
       </c>
-      <c r="S7">
+      <c r="U7">
         <v>6000</v>
       </c>
-      <c r="T7">
+      <c r="V7">
+        <f t="shared" si="3"/>
+        <v>3800</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="4"/>
+        <v>880</v>
+      </c>
+      <c r="X7">
         <v>2</v>
       </c>
-      <c r="U7">
+      <c r="Y7">
         <v>10</v>
       </c>
-      <c r="V7">
+      <c r="Z7">
         <v>100</v>
       </c>
-      <c r="W7">
+      <c r="AA7">
         <v>1000</v>
       </c>
-      <c r="X7">
-        <v>0</v>
-      </c>
-      <c r="Y7">
+      <c r="AB7">
+        <f t="shared" si="6"/>
+        <v>550</v>
+      </c>
+      <c r="AC7">
+        <f t="shared" si="7"/>
+        <v>180</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
         <v>7</v>
       </c>
-      <c r="Z7">
-        <v>0</v>
-      </c>
-      <c r="AA7">
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
         <v>500</v>
       </c>
-      <c r="AB7">
-        <v>0</v>
-      </c>
-      <c r="AC7">
+      <c r="AH7">
+        <f t="shared" si="8"/>
+        <v>250</v>
+      </c>
+      <c r="AI7">
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+      <c r="AK7">
         <v>3</v>
       </c>
-      <c r="AD7">
-        <v>0</v>
-      </c>
-      <c r="AE7">
+      <c r="AL7">
+        <v>0</v>
+      </c>
+      <c r="AM7">
         <v>300</v>
       </c>
+      <c r="AN7">
+        <f t="shared" si="11"/>
+        <v>150</v>
+      </c>
+      <c r="AO7">
+        <f t="shared" si="12"/>
+        <v>60</v>
+      </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1294,55 +1594,95 @@
         <v>7000</v>
       </c>
       <c r="P8">
+        <f t="shared" si="1"/>
+        <v>4250</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="2"/>
+        <v>1100</v>
+      </c>
+      <c r="R8">
         <v>20</v>
       </c>
-      <c r="Q8">
+      <c r="S8">
         <v>50</v>
       </c>
-      <c r="R8">
+      <c r="T8">
         <v>1000</v>
       </c>
-      <c r="S8">
+      <c r="U8">
         <v>4500</v>
       </c>
-      <c r="T8">
+      <c r="V8">
+        <f t="shared" si="3"/>
+        <v>2750</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="4"/>
+        <v>700</v>
+      </c>
+      <c r="X8">
         <v>2</v>
       </c>
-      <c r="U8">
+      <c r="Y8">
         <v>10</v>
       </c>
-      <c r="V8">
+      <c r="Z8">
         <v>100</v>
       </c>
-      <c r="W8">
+      <c r="AA8">
         <v>1000</v>
       </c>
-      <c r="X8">
-        <v>0</v>
-      </c>
-      <c r="Y8">
+      <c r="AB8">
+        <f t="shared" si="6"/>
+        <v>550</v>
+      </c>
+      <c r="AC8">
+        <f t="shared" si="7"/>
+        <v>180</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
         <v>7</v>
       </c>
-      <c r="Z8">
-        <v>0</v>
-      </c>
-      <c r="AA8">
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
         <v>500</v>
       </c>
-      <c r="AB8">
-        <v>0</v>
-      </c>
-      <c r="AC8">
+      <c r="AH8">
+        <f t="shared" si="8"/>
+        <v>250</v>
+      </c>
+      <c r="AI8">
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
+      <c r="AJ8">
+        <v>0</v>
+      </c>
+      <c r="AK8">
         <v>3</v>
       </c>
-      <c r="AD8">
-        <v>0</v>
-      </c>
-      <c r="AE8">
+      <c r="AL8">
+        <v>0</v>
+      </c>
+      <c r="AM8">
         <v>200</v>
       </c>
+      <c r="AN8">
+        <f t="shared" si="11"/>
+        <v>100</v>
+      </c>
+      <c r="AO8">
+        <f t="shared" si="12"/>
+        <v>40</v>
+      </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1371,95 +1711,135 @@
         <v>9</v>
       </c>
       <c r="J9">
-        <f t="shared" ref="J9:S10" si="3">J8</f>
+        <f t="shared" ref="J9:O10" si="13">J8</f>
         <v>3600</v>
       </c>
       <c r="K9">
+        <f t="shared" si="13"/>
+        <v>11000</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="13"/>
+        <v>70</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="13"/>
+        <v>1500</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="13"/>
+        <v>7000</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="1"/>
+        <v>4250</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="2"/>
+        <v>1100</v>
+      </c>
+      <c r="R9">
+        <f>R8</f>
+        <v>20</v>
+      </c>
+      <c r="S9">
+        <f>S8</f>
+        <v>50</v>
+      </c>
+      <c r="T9">
+        <f>T8</f>
+        <v>1000</v>
+      </c>
+      <c r="U9">
+        <f>U8</f>
+        <v>4500</v>
+      </c>
+      <c r="V9">
         <f t="shared" si="3"/>
-        <v>11000</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="3"/>
-        <v>70</v>
-      </c>
-      <c r="N9">
-        <f t="shared" si="3"/>
-        <v>1500</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="3"/>
-        <v>7000</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="3"/>
-        <v>50</v>
-      </c>
-      <c r="R9">
-        <f t="shared" si="3"/>
-        <v>1000</v>
-      </c>
-      <c r="S9">
-        <f t="shared" si="3"/>
-        <v>4500</v>
-      </c>
-      <c r="T9">
-        <f t="shared" ref="T9:AC10" si="4">T8</f>
-        <v>2</v>
-      </c>
-      <c r="U9">
-        <f t="shared" si="4"/>
-        <v>10</v>
-      </c>
-      <c r="V9">
-        <f t="shared" si="4"/>
-        <v>100</v>
+        <v>2750</v>
       </c>
       <c r="W9">
         <f t="shared" si="4"/>
+        <v>700</v>
+      </c>
+      <c r="X9">
+        <f t="shared" ref="X9:AG10" si="14">X8</f>
+        <v>2</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="14"/>
+        <v>100</v>
+      </c>
+      <c r="AA9">
+        <f t="shared" si="14"/>
         <v>1000</v>
       </c>
-      <c r="X9">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y9">
-        <f t="shared" si="4"/>
+      <c r="AB9">
+        <f t="shared" si="6"/>
+        <v>550</v>
+      </c>
+      <c r="AC9">
+        <f t="shared" si="7"/>
+        <v>180</v>
+      </c>
+      <c r="AD9">
+        <f>AD8</f>
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <f>AE8</f>
         <v>7</v>
       </c>
-      <c r="Z9">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AA9">
-        <f t="shared" si="4"/>
+      <c r="AF9">
+        <f>AF8</f>
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <f>AG8</f>
         <v>500</v>
       </c>
-      <c r="AB9">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AC9">
-        <f t="shared" si="4"/>
+      <c r="AH9">
+        <f t="shared" si="8"/>
+        <v>250</v>
+      </c>
+      <c r="AI9">
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
+      <c r="AJ9">
+        <f>AJ8</f>
+        <v>0</v>
+      </c>
+      <c r="AK9">
+        <f>AK8</f>
         <v>3</v>
       </c>
-      <c r="AD9">
-        <f t="shared" ref="AD9:AM10" si="5">AD8</f>
-        <v>0</v>
-      </c>
-      <c r="AE9">
-        <f t="shared" si="5"/>
+      <c r="AL9">
+        <f t="shared" ref="AL9:AM10" si="15">AL8</f>
+        <v>0</v>
+      </c>
+      <c r="AM9">
+        <f t="shared" si="15"/>
         <v>200</v>
       </c>
+      <c r="AN9">
+        <f t="shared" si="11"/>
+        <v>100</v>
+      </c>
+      <c r="AO9">
+        <f t="shared" si="12"/>
+        <v>40</v>
+      </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1488,92 +1868,132 @@
         <v>9</v>
       </c>
       <c r="J10">
+        <f t="shared" si="13"/>
+        <v>3600</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="13"/>
+        <v>11000</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="13"/>
+        <v>70</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="13"/>
+        <v>1500</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="13"/>
+        <v>7000</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="1"/>
+        <v>4250</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="2"/>
+        <v>1100</v>
+      </c>
+      <c r="R10">
+        <f>R9</f>
+        <v>20</v>
+      </c>
+      <c r="S10">
+        <f>S9</f>
+        <v>50</v>
+      </c>
+      <c r="T10">
+        <f>T9</f>
+        <v>1000</v>
+      </c>
+      <c r="U10">
+        <f>U9</f>
+        <v>4500</v>
+      </c>
+      <c r="V10">
         <f t="shared" si="3"/>
-        <v>3600</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="3"/>
-        <v>11000</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="3"/>
-        <v>70</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="3"/>
-        <v>1500</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="3"/>
-        <v>7000</v>
-      </c>
-      <c r="P10">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="3"/>
-        <v>50</v>
-      </c>
-      <c r="R10">
-        <f t="shared" si="3"/>
-        <v>1000</v>
-      </c>
-      <c r="S10">
-        <f t="shared" si="3"/>
-        <v>4500</v>
-      </c>
-      <c r="T10">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="U10">
-        <f t="shared" si="4"/>
-        <v>10</v>
-      </c>
-      <c r="V10">
-        <f t="shared" si="4"/>
-        <v>100</v>
+        <v>2750</v>
       </c>
       <c r="W10">
         <f t="shared" si="4"/>
+        <v>700</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="14"/>
+        <v>100</v>
+      </c>
+      <c r="AA10">
+        <f t="shared" si="14"/>
         <v>1000</v>
       </c>
-      <c r="X10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y10">
-        <f t="shared" si="4"/>
+      <c r="AB10">
+        <f t="shared" si="6"/>
+        <v>550</v>
+      </c>
+      <c r="AC10">
+        <f t="shared" si="7"/>
+        <v>180</v>
+      </c>
+      <c r="AD10">
+        <f>AD9</f>
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <f>AE9</f>
         <v>7</v>
       </c>
-      <c r="Z10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AA10">
-        <f t="shared" si="4"/>
+      <c r="AF10">
+        <f>AF9</f>
+        <v>0</v>
+      </c>
+      <c r="AG10">
+        <f>AG9</f>
         <v>500</v>
       </c>
-      <c r="AB10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AC10">
-        <f t="shared" si="4"/>
+      <c r="AH10">
+        <f t="shared" si="8"/>
+        <v>250</v>
+      </c>
+      <c r="AI10">
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
+      <c r="AJ10">
+        <f>AJ9</f>
+        <v>0</v>
+      </c>
+      <c r="AK10">
+        <f>AK9</f>
         <v>3</v>
       </c>
-      <c r="AD10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AE10">
-        <f t="shared" si="5"/>
+      <c r="AL10">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AM10">
+        <f t="shared" si="15"/>
         <v>200</v>
+      </c>
+      <c r="AN10">
+        <f t="shared" si="11"/>
+        <v>100</v>
+      </c>
+      <c r="AO10">
+        <f t="shared" si="12"/>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>